<commit_message>
modify event filter student timetable
</commit_message>
<xml_diff>
--- a/studMin/TemplateExcel/schedule_all_teacher.xlsx
+++ b/studMin/TemplateExcel/schedule_all_teacher.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khoi\Documents\GitHub\studMin\studMin\TemplateExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81F77BE-9F91-48C2-A488-94760A2EDAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE80E010-8412-41FB-90C0-C9D3C82754C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>School</t>
   </si>
@@ -73,10 +73,6 @@
   </si>
   <si>
     <t>10A3</t>
-  </si>
-  <si>
-    <t>Anh
-Nguyễn Hoàng Lân</t>
   </si>
   <si>
     <t>Toán
@@ -91,10 +87,6 @@
 Lý Hoàng Phi</t>
   </si>
   <si>
-    <t>Hóa
-Hoàng Xuân Trường</t>
-  </si>
-  <si>
     <t>Địa
 Nguyễn Võ Thanh Minh</t>
   </si>
@@ -123,8 +115,16 @@
 Trần Phan Anh Đức</t>
   </si>
   <si>
-    <t>GDCN
+    <t>Hóa
+Hoàng Vũ</t>
+  </si>
+  <si>
+    <t>GDCD
 Phạm Võ Anh Thi</t>
+  </si>
+  <si>
+    <t>Anh
+Nguyễn Xuân Tài</t>
   </si>
 </sst>
 </file>
@@ -173,7 +173,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +192,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -432,11 +438,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -468,12 +487,15 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -495,14 +517,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -807,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -853,55 +875,55 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="29">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="30">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="29">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="30">
         <v>3</v>
       </c>
       <c r="D8" s="11"/>
@@ -909,57 +931,57 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="29">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="30">
         <v>4</v>
       </c>
       <c r="D10" s="11"/>
-      <c r="E10" s="18" t="s">
-        <v>19</v>
+      <c r="E10" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="29"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="16"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="29">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="30">
         <v>5</v>
       </c>
       <c r="D12" s="11"/>
-      <c r="E12" s="16"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="30"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="19"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="29">
         <v>1</v>
       </c>
       <c r="D14" s="12"/>
@@ -967,17 +989,17 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="29"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="29">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="30">
         <v>2</v>
       </c>
       <c r="D16" s="11"/>
@@ -985,55 +1007,55 @@
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="29"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="29">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="30">
         <v>3</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="29"/>
+    <row r="19" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="29">
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="30">
         <v>4</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="24"/>
+      <c r="F20" s="22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="29"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="29">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="30">
         <v>5</v>
       </c>
       <c r="D22" s="11"/>
@@ -1041,63 +1063,63 @@
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="31"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="29">
         <v>1</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>21</v>
+      <c r="D24" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="E24" s="12"/>
-      <c r="F24" s="15" t="s">
-        <v>22</v>
+      <c r="F24" s="16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="17"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="11"/>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="29">
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="30">
         <v>2</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="13" t="s">
-        <v>23</v>
+      <c r="F26" s="23" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="29"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="9"/>
+      <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="29">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="30">
         <v>3</v>
       </c>
       <c r="D28" s="11"/>
@@ -1105,17 +1127,17 @@
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="29"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="29">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="30">
         <v>4</v>
       </c>
       <c r="D30" s="11"/>
@@ -1123,17 +1145,17 @@
       <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="29"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="29">
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="30">
         <v>5</v>
       </c>
       <c r="D32" s="11"/>
@@ -1141,79 +1163,79 @@
       <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="30"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="31"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="25" t="s">
+      <c r="A34" s="27"/>
+      <c r="B34" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="28">
+      <c r="C34" s="29">
         <v>1</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="30">
+        <v>2</v>
+      </c>
+      <c r="D36" s="17"/>
+      <c r="E36" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="21"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="29">
-        <v>2</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="F36" s="22"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="21"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="22"/>
     </row>
     <row r="38" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="29">
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="30">
         <v>3</v>
       </c>
       <c r="D38" s="11"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="21"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="22"/>
     </row>
     <row r="39" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="29"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="21"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="22"/>
     </row>
     <row r="40" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="29">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="30">
         <v>4</v>
       </c>
       <c r="D40" s="11"/>
@@ -1221,17 +1243,17 @@
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="29"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="29">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="30">
         <v>5</v>
       </c>
       <c r="D42" s="11"/>
@@ -1239,21 +1261,21 @@
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="31"/>
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="32"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C44" s="29">
         <v>1</v>
       </c>
       <c r="D44" s="12"/>
@@ -1261,17 +1283,17 @@
       <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="29"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="29">
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="30">
         <v>2</v>
       </c>
       <c r="D46" s="11"/>
@@ -1279,17 +1301,17 @@
       <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="29"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="29">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="30">
         <v>3</v>
       </c>
       <c r="D48" s="11"/>
@@ -1297,17 +1319,17 @@
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="29"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="30"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="29">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="30">
         <v>4</v>
       </c>
       <c r="D50" s="11"/>
@@ -1315,17 +1337,17 @@
       <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="29"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="30"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="29">
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="30">
         <v>5</v>
       </c>
       <c r="D52" s="11"/>
@@ -1333,57 +1355,57 @@
       <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="30"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="31"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="25" t="s">
+      <c r="A54" s="27"/>
+      <c r="B54" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="28">
+      <c r="C54" s="29">
         <v>1</v>
       </c>
-      <c r="D54" s="15" t="s">
-        <v>27</v>
+      <c r="D54" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="16"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="17"/>
       <c r="E55" s="11"/>
       <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="29">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="30">
         <v>2</v>
       </c>
-      <c r="D56" s="16"/>
+      <c r="D56" s="17"/>
       <c r="E56" s="11"/>
       <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="17"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="18"/>
       <c r="E57" s="11"/>
       <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="29">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="30">
         <v>3</v>
       </c>
       <c r="D58" s="11"/>
@@ -1391,17 +1413,17 @@
       <c r="F58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="29"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="30"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
       <c r="F59" s="9"/>
     </row>
     <row r="60" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="29">
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="30">
         <v>4</v>
       </c>
       <c r="D60" s="11"/>
@@ -1409,41 +1431,41 @@
       <c r="F60" s="9"/>
     </row>
     <row r="61" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="29"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="30"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="9"/>
     </row>
     <row r="62" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="29">
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="30">
         <v>5</v>
       </c>
-      <c r="D62" s="18" t="s">
-        <v>28</v>
+      <c r="D62" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="E62" s="11"/>
       <c r="F62" s="9"/>
     </row>
     <row r="63" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="27"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="19"/>
+      <c r="A63" s="28"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="20"/>
       <c r="E63" s="11"/>
       <c r="F63" s="10"/>
     </row>
     <row r="64" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
+      <c r="A64" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="28">
+      <c r="C64" s="29">
         <v>1</v>
       </c>
       <c r="D64" s="12"/>
@@ -1451,17 +1473,17 @@
       <c r="F64" s="8"/>
     </row>
     <row r="65" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A65" s="26"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="29"/>
+      <c r="A65" s="27"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="30"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
       <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A66" s="26"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="29">
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="30">
         <v>2</v>
       </c>
       <c r="D66" s="11"/>
@@ -1469,17 +1491,17 @@
       <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A67" s="26"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="29"/>
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="30"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
       <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="29">
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="30">
         <v>3</v>
       </c>
       <c r="D68" s="11"/>
@@ -1487,17 +1509,17 @@
       <c r="F68" s="9"/>
     </row>
     <row r="69" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A69" s="26"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="29"/>
+      <c r="A69" s="27"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="30"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
       <c r="F69" s="9"/>
     </row>
     <row r="70" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="29">
+      <c r="A70" s="27"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="30">
         <v>4</v>
       </c>
       <c r="D70" s="11"/>
@@ -1505,17 +1527,17 @@
       <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="29"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="30"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
       <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="29">
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="30">
         <v>5</v>
       </c>
       <c r="D72" s="11"/>
@@ -1523,19 +1545,19 @@
       <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="26"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="30"/>
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="31"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
       <c r="F73" s="9"/>
     </row>
     <row r="74" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
-      <c r="B74" s="25" t="s">
+      <c r="A74" s="27"/>
+      <c r="B74" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="28">
+      <c r="C74" s="29">
         <v>1</v>
       </c>
       <c r="D74" s="12"/>
@@ -1543,17 +1565,17 @@
       <c r="F74" s="8"/>
     </row>
     <row r="75" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A75" s="26"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="29"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="30"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
       <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="29">
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="30">
         <v>2</v>
       </c>
       <c r="D76" s="11"/>
@@ -1561,17 +1583,17 @@
       <c r="F76" s="9"/>
     </row>
     <row r="77" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A77" s="26"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="29"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="30"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
       <c r="F77" s="9"/>
     </row>
     <row r="78" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="29">
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="30">
         <v>3</v>
       </c>
       <c r="D78" s="11"/>
@@ -1579,17 +1601,17 @@
       <c r="F78" s="9"/>
     </row>
     <row r="79" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A79" s="26"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="29"/>
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="30"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="29">
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="30">
         <v>4</v>
       </c>
       <c r="D80" s="11"/>
@@ -1597,17 +1619,17 @@
       <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="29"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="30"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
       <c r="F81" s="9"/>
     </row>
     <row r="82" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="29">
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="30">
         <v>5</v>
       </c>
       <c r="D82" s="11"/>
@@ -1615,21 +1637,21 @@
       <c r="F82" s="9"/>
     </row>
     <row r="83" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="31"/>
+      <c r="A83" s="28"/>
+      <c r="B83" s="28"/>
+      <c r="C83" s="32"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
       <c r="F83" s="10"/>
     </row>
     <row r="84" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A84" s="25" t="s">
+      <c r="A84" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B84" s="25" t="s">
+      <c r="B84" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C84" s="28">
+      <c r="C84" s="29">
         <v>1</v>
       </c>
       <c r="D84" s="12"/>
@@ -1637,17 +1659,17 @@
       <c r="F84" s="8"/>
     </row>
     <row r="85" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
-      <c r="B85" s="26"/>
-      <c r="C85" s="29"/>
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="30"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
       <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A86" s="26"/>
-      <c r="B86" s="26"/>
-      <c r="C86" s="29">
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="30">
         <v>2</v>
       </c>
       <c r="D86" s="11"/>
@@ -1655,17 +1677,17 @@
       <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="29"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="30"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
       <c r="F87" s="9"/>
     </row>
     <row r="88" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
-      <c r="B88" s="26"/>
-      <c r="C88" s="29">
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="30">
         <v>3</v>
       </c>
       <c r="D88" s="11"/>
@@ -1673,17 +1695,17 @@
       <c r="F88" s="9"/>
     </row>
     <row r="89" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
-      <c r="B89" s="26"/>
-      <c r="C89" s="29"/>
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="30"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
       <c r="F89" s="9"/>
     </row>
     <row r="90" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A90" s="26"/>
-      <c r="B90" s="26"/>
-      <c r="C90" s="29">
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="30">
         <v>4</v>
       </c>
       <c r="D90" s="11"/>
@@ -1691,17 +1713,17 @@
       <c r="F90" s="9"/>
     </row>
     <row r="91" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
-      <c r="B91" s="26"/>
-      <c r="C91" s="29"/>
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="30"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
       <c r="F91" s="9"/>
     </row>
     <row r="92" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A92" s="26"/>
-      <c r="B92" s="26"/>
-      <c r="C92" s="29">
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="30">
         <v>5</v>
       </c>
       <c r="D92" s="11"/>
@@ -1709,19 +1731,19 @@
       <c r="F92" s="9"/>
     </row>
     <row r="93" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="26"/>
-      <c r="B93" s="26"/>
-      <c r="C93" s="30"/>
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="31"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
       <c r="F93" s="9"/>
     </row>
     <row r="94" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
-      <c r="B94" s="25" t="s">
+      <c r="A94" s="27"/>
+      <c r="B94" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C94" s="28">
+      <c r="C94" s="29">
         <v>1</v>
       </c>
       <c r="D94" s="12"/>
@@ -1729,17 +1751,17 @@
       <c r="F94" s="8"/>
     </row>
     <row r="95" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
-      <c r="B95" s="26"/>
-      <c r="C95" s="29"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="30"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
       <c r="F95" s="9"/>
     </row>
     <row r="96" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A96" s="26"/>
-      <c r="B96" s="26"/>
-      <c r="C96" s="29">
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="30">
         <v>2</v>
       </c>
       <c r="D96" s="11"/>
@@ -1747,17 +1769,17 @@
       <c r="F96" s="9"/>
     </row>
     <row r="97" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="29"/>
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="30"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
       <c r="F97" s="9"/>
     </row>
     <row r="98" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
-      <c r="C98" s="29">
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="30">
         <v>3</v>
       </c>
       <c r="D98" s="11"/>
@@ -1765,17 +1787,17 @@
       <c r="F98" s="9"/>
     </row>
     <row r="99" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A99" s="26"/>
-      <c r="B99" s="26"/>
-      <c r="C99" s="29"/>
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="30"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
       <c r="F99" s="9"/>
     </row>
     <row r="100" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A100" s="26"/>
-      <c r="B100" s="26"/>
-      <c r="C100" s="29">
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="30">
         <v>4</v>
       </c>
       <c r="D100" s="11"/>
@@ -1783,17 +1805,17 @@
       <c r="F100" s="9"/>
     </row>
     <row r="101" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A101" s="26"/>
-      <c r="B101" s="26"/>
-      <c r="C101" s="29"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="30"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
       <c r="F101" s="9"/>
     </row>
     <row r="102" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
-      <c r="B102" s="26"/>
-      <c r="C102" s="29">
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="30">
         <v>5</v>
       </c>
       <c r="D102" s="11"/>
@@ -1801,39 +1823,41 @@
       <c r="F102" s="9"/>
     </row>
     <row r="103" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="27"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="31"/>
+      <c r="A103" s="28"/>
+      <c r="B103" s="28"/>
+      <c r="C103" s="32"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
       <c r="F103" s="10"/>
     </row>
-    <row r="104" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A104" s="25" t="s">
+    <row r="104" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B104" s="25" t="s">
+      <c r="B104" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="28">
+      <c r="C104" s="29">
         <v>1</v>
       </c>
-      <c r="D104" s="12"/>
+      <c r="D104" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="E104" s="12"/>
       <c r="F104" s="8"/>
     </row>
     <row r="105" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
-      <c r="B105" s="26"/>
-      <c r="C105" s="29"/>
-      <c r="D105" s="11"/>
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
+      <c r="C105" s="30"/>
+      <c r="D105" s="15"/>
       <c r="E105" s="11"/>
       <c r="F105" s="9"/>
     </row>
     <row r="106" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A106" s="26"/>
-      <c r="B106" s="26"/>
-      <c r="C106" s="29">
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="30">
         <v>2</v>
       </c>
       <c r="D106" s="11"/>
@@ -1841,17 +1865,17 @@
       <c r="F106" s="9"/>
     </row>
     <row r="107" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A107" s="26"/>
-      <c r="B107" s="26"/>
-      <c r="C107" s="29"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="30"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
       <c r="F107" s="9"/>
     </row>
     <row r="108" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
-      <c r="B108" s="26"/>
-      <c r="C108" s="29">
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="30">
         <v>3</v>
       </c>
       <c r="D108" s="11"/>
@@ -1859,17 +1883,17 @@
       <c r="F108" s="9"/>
     </row>
     <row r="109" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A109" s="26"/>
-      <c r="B109" s="26"/>
-      <c r="C109" s="29"/>
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="30"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
       <c r="F109" s="9"/>
     </row>
     <row r="110" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A110" s="26"/>
-      <c r="B110" s="26"/>
-      <c r="C110" s="29">
+      <c r="A110" s="27"/>
+      <c r="B110" s="27"/>
+      <c r="C110" s="30">
         <v>4</v>
       </c>
       <c r="D110" s="11"/>
@@ -1877,17 +1901,17 @@
       <c r="F110" s="9"/>
     </row>
     <row r="111" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
-      <c r="B111" s="26"/>
-      <c r="C111" s="29"/>
+      <c r="A111" s="27"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="30"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
       <c r="F111" s="9"/>
     </row>
     <row r="112" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
-      <c r="B112" s="26"/>
-      <c r="C112" s="29">
+      <c r="A112" s="27"/>
+      <c r="B112" s="27"/>
+      <c r="C112" s="30">
         <v>5</v>
       </c>
       <c r="D112" s="11"/>
@@ -1895,19 +1919,19 @@
       <c r="F112" s="9"/>
     </row>
     <row r="113" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="26"/>
-      <c r="B113" s="26"/>
-      <c r="C113" s="30"/>
+      <c r="A113" s="27"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="31"/>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
       <c r="F113" s="9"/>
     </row>
     <row r="114" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A114" s="26"/>
-      <c r="B114" s="25" t="s">
+      <c r="A114" s="27"/>
+      <c r="B114" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C114" s="28">
+      <c r="C114" s="29">
         <v>1</v>
       </c>
       <c r="D114" s="12"/>
@@ -1915,17 +1939,17 @@
       <c r="F114" s="8"/>
     </row>
     <row r="115" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A115" s="26"/>
-      <c r="B115" s="26"/>
-      <c r="C115" s="29"/>
+      <c r="A115" s="27"/>
+      <c r="B115" s="27"/>
+      <c r="C115" s="30"/>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
       <c r="F115" s="9"/>
     </row>
     <row r="116" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A116" s="26"/>
-      <c r="B116" s="26"/>
-      <c r="C116" s="29">
+      <c r="A116" s="27"/>
+      <c r="B116" s="27"/>
+      <c r="C116" s="30">
         <v>2</v>
       </c>
       <c r="D116" s="11"/>
@@ -1933,17 +1957,17 @@
       <c r="F116" s="9"/>
     </row>
     <row r="117" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A117" s="26"/>
-      <c r="B117" s="26"/>
-      <c r="C117" s="29"/>
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="30"/>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
       <c r="F117" s="9"/>
     </row>
     <row r="118" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A118" s="26"/>
-      <c r="B118" s="26"/>
-      <c r="C118" s="29">
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
+      <c r="C118" s="30">
         <v>3</v>
       </c>
       <c r="D118" s="11"/>
@@ -1951,17 +1975,17 @@
       <c r="F118" s="9"/>
     </row>
     <row r="119" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A119" s="26"/>
-      <c r="B119" s="26"/>
-      <c r="C119" s="29"/>
+      <c r="A119" s="27"/>
+      <c r="B119" s="27"/>
+      <c r="C119" s="30"/>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
       <c r="F119" s="9"/>
     </row>
     <row r="120" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A120" s="26"/>
-      <c r="B120" s="26"/>
-      <c r="C120" s="29">
+      <c r="A120" s="27"/>
+      <c r="B120" s="27"/>
+      <c r="C120" s="30">
         <v>4</v>
       </c>
       <c r="D120" s="11"/>
@@ -1969,17 +1993,17 @@
       <c r="F120" s="9"/>
     </row>
     <row r="121" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A121" s="26"/>
-      <c r="B121" s="26"/>
-      <c r="C121" s="29"/>
+      <c r="A121" s="27"/>
+      <c r="B121" s="27"/>
+      <c r="C121" s="30"/>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
       <c r="F121" s="9"/>
     </row>
     <row r="122" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A122" s="26"/>
-      <c r="B122" s="26"/>
-      <c r="C122" s="29">
+      <c r="A122" s="27"/>
+      <c r="B122" s="27"/>
+      <c r="C122" s="30">
         <v>5</v>
       </c>
       <c r="D122" s="11"/>
@@ -1987,15 +2011,15 @@
       <c r="F122" s="9"/>
     </row>
     <row r="123" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="27"/>
-      <c r="B123" s="27"/>
-      <c r="C123" s="31"/>
-      <c r="D123" s="14"/>
-      <c r="E123" s="14"/>
+      <c r="A123" s="28"/>
+      <c r="B123" s="28"/>
+      <c r="C123" s="32"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
       <c r="F123" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="90">
+  <mergeCells count="92">
     <mergeCell ref="A84:A103"/>
     <mergeCell ref="B84:B93"/>
     <mergeCell ref="C84:C85"/>
@@ -2078,7 +2102,8 @@
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="F4:F7"/>
     <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="D104:D105"/>
     <mergeCell ref="D54:D57"/>
     <mergeCell ref="D62:D63"/>
     <mergeCell ref="D24:D25"/>
@@ -2086,6 +2111,7 @@
     <mergeCell ref="D34:D37"/>
     <mergeCell ref="F34:F39"/>
     <mergeCell ref="E36:E39"/>
+    <mergeCell ref="F26:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>